<commit_message>
Audit improvement plan fixes
</commit_message>
<xml_diff>
--- a/src/private/templates/auditor_improvement_plan.xlsx
+++ b/src/private/templates/auditor_improvement_plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,24 +31,12 @@
     <t>Supplier Improvement Plan</t>
   </si>
   <si>
-    <t>SUPPLIER NAME</t>
-  </si>
-  <si>
     <t>GLOBAL WELDING MONGOLIA</t>
   </si>
   <si>
-    <t>AUDIT DATE</t>
-  </si>
-  <si>
     <t>MARCH 30,2017</t>
   </si>
   <si>
-    <t>PLANNED REVIEW DATE</t>
-  </si>
-  <si>
-    <t>QUALIFICATION AUDITOR(S) NAME(S)</t>
-  </si>
-  <si>
     <t>NARANTSATSRAL GONCHIG</t>
   </si>
   <si>
@@ -62,13 +50,25 @@
   </si>
   <si>
     <t>REQUIRED ACTION</t>
+  </si>
+  <si>
+    <t>Supplier name</t>
+  </si>
+  <si>
+    <t>Audit date</t>
+  </si>
+  <si>
+    <t>Planned review date</t>
+  </si>
+  <si>
+    <t>Qualification auditor(s) name(s)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,8 +87,19 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -98,6 +109,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7DEE8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -173,11 +196,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -186,28 +210,28 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -216,6 +240,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFB7DEE8"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -261,8 +290,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="609601" y="190501"/>
-          <a:ext cx="1495423" cy="618796"/>
+          <a:off x="669637" y="177031"/>
+          <a:ext cx="1619345" cy="624569"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -574,7 +603,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="165" zoomScalePageLayoutView="165" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E2" sqref="E2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -593,137 +622,137 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="13" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="4"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="4"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="B7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
-      <c r="B8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5">
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6">
         <v>42889</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
-      <c r="B9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
@@ -741,45 +770,45 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
-      <c r="B11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="6"/>
+      <c r="B11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="11"/>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
       <c r="K12" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F2:H3"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E6:J6"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E2:I3"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="E8:J8"/>
     <mergeCell ref="B9:D9"/>

</xml_diff>

<commit_message>
update improvement plan template
</commit_message>
<xml_diff>
--- a/src/private/templates/auditor_improvement_plan.xlsx
+++ b/src/private/templates/auditor_improvement_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/batamar/Documents/works/ot-backend/src/private/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C739E946-91D7-C743-BB5D-BF026B0DCA7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981FF17F-9B05-4549-B712-0470DD78D42A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="12"/>
       <color theme="8" tint="-0.249977111117893"/>
       <name val="Verdana"/>
       <family val="2"/>
@@ -244,47 +244,47 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -691,7 +691,7 @@
   <dimension ref="B1:J6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="82" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5"/>
+      <selection activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -707,96 +707,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:J3"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E6:J6"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E4:J4"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:J2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>